<commit_message>
change manage order import template file
</commit_message>
<xml_diff>
--- a/resources/manage/assets/xlsx/发货模板.xlsx
+++ b/resources/manage/assets/xlsx/发货模板.xlsx
@@ -701,13 +701,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1238,14 +1238,15 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="5" width="22.875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.875" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="9" style="1"/>
+    <col min="1" max="1" width="22.875" style="1" customWidth="1"/>
+    <col min="2" max="5" width="22.875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="22.875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
     <row r="1" ht="108" customHeight="1" spans="1:1">
@@ -1257,22 +1258,22 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>